<commit_message>
Cambios en productbacklog plus html estrucutra Fabiola Benitez
</commit_message>
<xml_diff>
--- a/Documentacion Proyecto/ProductBacklog.xlsx
+++ b/Documentacion Proyecto/ProductBacklog.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FABIOLA\Desktop\Respositorio FS Final\Proyecto-Fullstack-ISPC-G1\Documentacion Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FABIOLA\Desktop\Proyecto FS  Final Corregido\Proyecto-Fullstack-ISPC-G1\Documentacion Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>No. Historia de usuario</t>
   </si>
@@ -93,78 +93,21 @@
     <t xml:space="preserve">Usuario </t>
   </si>
   <si>
-    <t>Observaciones</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Datos del Producto: Nombre, Descripción, Stock Minino, Tipo de Producto,
-Unidad de Medida, Moneda y Depósito.
-</t>
-  </si>
-  <si>
     <t>Eliminar un producto existente.</t>
   </si>
   <si>
     <t>Buscar informacion relevante de un producto</t>
   </si>
   <si>
-    <t>Registrar el alta de un proveedor que se incorpora a la nómina, con los datos propios del mismo.</t>
-  </si>
-  <si>
-    <t>Mantener un registro de proveedores actualizado</t>
-  </si>
-  <si>
-    <t>) Datos del Proveedor: Nombre, CUIT, Mail, Dirección, Teléfono, y Descripción.</t>
-  </si>
-  <si>
-    <t>Modificar una o varias características de un proveedor ya registrado en el sistema. Descripción</t>
-  </si>
-  <si>
-    <t>Eliminar un proveedor existente</t>
-  </si>
-  <si>
-    <t>Consultar un producto proveedor existente.</t>
-  </si>
-  <si>
-    <t>Registrar un nuevo pedido</t>
-  </si>
-  <si>
     <t>Mantener un registro de pedidos  actualizado</t>
   </si>
   <si>
-    <t>Modificar una o varias productos de un pedido ya registrado en el sistema.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Eliminar un pedido ya registrado en el sistema.</t>
-  </si>
-  <si>
-    <t>Consultar uno o más pedidos ya registrados en el sistema.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Consultar el Stock Actual registrado en el sistema.</t>
-  </si>
-  <si>
-    <t>Generar informes de stock actualizados</t>
-  </si>
-  <si>
-    <t>Datos del Producto: Nombre, Stock Disponible y Stock Real. Dentro del producto se encuentran los siguientes datos: Numero de remito, tipo de movimiento, ingreso y egreso.</t>
-  </si>
-  <si>
     <t>Actualizar el Stock Actual registrado en el sistema.</t>
   </si>
   <si>
-    <t>Obtener informes según diferentes filtros.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Conocer la situacion general del stock </t>
   </si>
   <si>
-    <t>1) Datos del producto: nombre, tipo de producto, unidad de medida, deposito,
-stock mínimo, stock disponible y stock real.</t>
-  </si>
-  <si>
-    <t>Datos del Pedido: Cliente, Remito, N de Factura, Descripción, Retirado por, Deposito, Distribución y Estado. Producto y Cantidad.</t>
-  </si>
-  <si>
     <t>US001</t>
   </si>
   <si>
@@ -201,21 +144,6 @@
     <t>US0012</t>
   </si>
   <si>
-    <t>US0013</t>
-  </si>
-  <si>
-    <t>US0014</t>
-  </si>
-  <si>
-    <t>US0015</t>
-  </si>
-  <si>
-    <t>Consultar un producto existsente.</t>
-  </si>
-  <si>
-    <t>US0016</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quiero darme de alta en el sistemas </t>
   </si>
   <si>
@@ -228,37 +156,34 @@
     <t xml:space="preserve">Poder ingresar con mi clave nueva al sistema de gestion </t>
   </si>
   <si>
-    <t>US0017</t>
-  </si>
-  <si>
-    <t>US0018</t>
-  </si>
-  <si>
-    <t>US0019</t>
-  </si>
-  <si>
     <t>Quiero acceder al sistema de gestion con mi usuario</t>
   </si>
   <si>
     <t>Poder realizar las gestiones oportunas en el sistema</t>
   </si>
   <si>
-    <t>Control de stock, generacion de informe, carga de datos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acceso al sistema desde perfil de cuenta de usuario </t>
-  </si>
-  <si>
-    <t>quiero suscribirme al boletin de novedades mensual  por medio del sitio web.</t>
-  </si>
-  <si>
-    <t>Para mantenerme informado de las noticias del sistema de gestion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suscripcion a boletin de novedades mensual </t>
-  </si>
-  <si>
     <t xml:space="preserve">Modificar una o varias características de un producto ya registrado en el sistema. </t>
+  </si>
+  <si>
+    <t>Registrar una venta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Listar los 5 productos mas vendidos </t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtener los productos que son mas vendidos </t>
+  </si>
+  <si>
+    <t>Consultar el Stock Actual registrado en el sistema.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Obtener los productos que tienen poco stock minimo </t>
+  </si>
+  <si>
+    <t>mantener un registro de productos con stock minimo para reponer</t>
+  </si>
+  <si>
+    <t>Consultar un producto existente.</t>
   </si>
 </sst>
 </file>
@@ -366,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -387,35 +312,20 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:K65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -767,10 +677,9 @@
     <col min="2" max="2" width="37.125" customWidth="1"/>
     <col min="3" max="3" width="81.5" customWidth="1"/>
     <col min="4" max="4" width="63.875" customWidth="1"/>
-    <col min="5" max="5" width="143.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -782,10 +691,9 @@
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-    </row>
-    <row r="2" spans="1:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+    </row>
+    <row r="2" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="4"/>
@@ -798,9 +706,8 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -812,9 +719,8 @@
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -826,9 +732,8 @@
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" ht="37.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:11" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -841,474 +746,358 @@
       <c r="D5" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="7" t="s">
-        <v>9</v>
-      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="15" t="s">
-        <v>10</v>
-      </c>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="13" t="s">
+      <c r="C7" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="15" t="s">
-        <v>10</v>
-      </c>
+      <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="13" t="s">
+      <c r="C8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="15" t="s">
-        <v>10</v>
-      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="15" t="s">
+      <c r="C9" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="10" t="s">
         <v>10</v>
       </c>
+      <c r="E9" s="4"/>
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="16" t="s">
-        <v>15</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="4"/>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="16" t="s">
-        <v>15</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="4"/>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>15</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="4"/>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-      <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="16" t="s">
-        <v>15</v>
-      </c>
+      <c r="C13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="4"/>
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
-      <c r="L13" s="4"/>
-    </row>
-    <row r="14" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="16" t="s">
-        <v>31</v>
-      </c>
+      <c r="C14" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4"/>
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="16" t="s">
-        <v>31</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="4"/>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-      <c r="L15" s="4"/>
-    </row>
-    <row r="16" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C16" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>31</v>
-      </c>
+      <c r="C16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-    </row>
-    <row r="17" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" s="16" t="s">
+      <c r="C17" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>31</v>
       </c>
+      <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="4"/>
-    </row>
-    <row r="18" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E18" s="16" t="s">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="18" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-    </row>
-    <row r="19" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>26</v>
-      </c>
+    </row>
+    <row r="19" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-    </row>
-    <row r="20" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>30</v>
-      </c>
+    </row>
+    <row r="20" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-    </row>
-    <row r="21" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>59</v>
-      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-    </row>
-    <row r="22" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="E22" s="13" t="s">
-        <v>59</v>
-      </c>
+    </row>
+    <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="4"/>
-    </row>
-    <row r="23" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="E23" s="13" t="s">
-        <v>58</v>
-      </c>
+    </row>
+    <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4"/>
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-    </row>
-    <row r="24" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>62</v>
-      </c>
+    </row>
+    <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-    </row>
-    <row r="25" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1320,10 +1109,9 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-    </row>
-    <row r="26" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="10"/>
+    </row>
+    <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -1334,9 +1122,8 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="4"/>
-    </row>
-    <row r="27" spans="1:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1348,9 +1135,8 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="4"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1362,9 +1148,8 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="4"/>
-    </row>
-    <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1376,9 +1161,8 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="4"/>
-    </row>
-    <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1390,9 +1174,8 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="4"/>
-    </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1404,9 +1187,8 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="4"/>
-    </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1418,9 +1200,8 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="4"/>
-    </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1432,9 +1213,8 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1446,9 +1226,8 @@
       <c r="I34" s="4"/>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1460,9 +1239,8 @@
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
       <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1474,9 +1252,8 @@
       <c r="I36" s="4"/>
       <c r="J36" s="4"/>
       <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1488,9 +1265,8 @@
       <c r="I37" s="4"/>
       <c r="J37" s="4"/>
       <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1502,9 +1278,8 @@
       <c r="I38" s="4"/>
       <c r="J38" s="4"/>
       <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1516,9 +1291,8 @@
       <c r="I39" s="4"/>
       <c r="J39" s="4"/>
       <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1530,9 +1304,8 @@
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
-      <c r="L40" s="4"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1544,9 +1317,8 @@
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
-      <c r="L41" s="4"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1558,9 +1330,8 @@
       <c r="I42" s="4"/>
       <c r="J42" s="4"/>
       <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -1572,9 +1343,8 @@
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -1586,9 +1356,8 @@
       <c r="I44" s="4"/>
       <c r="J44" s="4"/>
       <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -1600,9 +1369,8 @@
       <c r="I45" s="4"/>
       <c r="J45" s="4"/>
       <c r="K45" s="4"/>
-      <c r="L45" s="4"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="4"/>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -1614,9 +1382,8 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="4"/>
       <c r="B47" s="4"/>
       <c r="C47" s="4"/>
@@ -1628,9 +1395,8 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="4"/>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -1642,9 +1408,8 @@
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
       <c r="K48" s="4"/>
-      <c r="L48" s="4"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="4"/>
       <c r="B49" s="4"/>
       <c r="C49" s="4"/>
@@ -1656,9 +1421,8 @@
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
       <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="4"/>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -1670,9 +1434,8 @@
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
       <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="4"/>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -1684,9 +1447,8 @@
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
       <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -1698,9 +1460,8 @@
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="4"/>
-      <c r="L52" s="4"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="4"/>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -1712,9 +1473,8 @@
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
       <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="4"/>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -1726,9 +1486,8 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="4"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -1740,9 +1499,8 @@
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -1754,9 +1512,8 @@
       <c r="I56" s="4"/>
       <c r="J56" s="4"/>
       <c r="K56" s="4"/>
-      <c r="L56" s="4"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -1768,9 +1525,8 @@
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
-      <c r="L57" s="4"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
@@ -1782,13 +1538,8 @@
       <c r="I58" s="4"/>
       <c r="J58" s="4"/>
       <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A59" s="4"/>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E59" s="4"/>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
@@ -1796,13 +1547,8 @@
       <c r="I59" s="4"/>
       <c r="J59" s="4"/>
       <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -1810,13 +1556,8 @@
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="4"/>
-      <c r="L60" s="4"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -1824,13 +1565,8 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
-      <c r="L61" s="4"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E62" s="4"/>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -1838,13 +1574,8 @@
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E63" s="4"/>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -1852,13 +1583,8 @@
       <c r="I63" s="4"/>
       <c r="J63" s="4"/>
       <c r="K63" s="4"/>
-      <c r="L63" s="4"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E64" s="4"/>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -1866,13 +1592,8 @@
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
-      <c r="L64" s="4"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
+    </row>
+    <row r="65" spans="5:11" x14ac:dyDescent="0.25">
       <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -1880,70 +1601,6 @@
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
       <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F66" s="4"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
-      <c r="J66" s="4"/>
-      <c r="K66" s="4"/>
-      <c r="L66" s="4"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F67" s="4"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
-      <c r="J67" s="4"/>
-      <c r="K67" s="4"/>
-      <c r="L67" s="4"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F68" s="4"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F69" s="4"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
-      <c r="J69" s="4"/>
-      <c r="K69" s="4"/>
-      <c r="L69" s="4"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F70" s="4"/>
-      <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
-      <c r="L71" s="4"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4"/>
-      <c r="L72" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Product Backlog - Diagrama de Ojetos y Clases en Python - fbenitez
</commit_message>
<xml_diff>
--- a/Documentacion Proyecto/ProductBacklog.xlsx
+++ b/Documentacion Proyecto/ProductBacklog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="64">
   <si>
     <t>No. Historia de usuario</t>
   </si>
@@ -87,27 +87,15 @@
     <t>Registrar el alta de un producto que se incorpora a la nómina, con los datos propios del mismo.</t>
   </si>
   <si>
-    <t>Mantenerse un stock de productos actualizado</t>
-  </si>
-  <si>
     <t xml:space="preserve">Usuario </t>
   </si>
   <si>
     <t>Eliminar un producto existente.</t>
   </si>
   <si>
-    <t>Buscar informacion relevante de un producto</t>
-  </si>
-  <si>
-    <t>Mantener un registro de pedidos  actualizado</t>
-  </si>
-  <si>
     <t>Actualizar el Stock Actual registrado en el sistema.</t>
   </si>
   <si>
-    <t xml:space="preserve">Conocer la situacion general del stock </t>
-  </si>
-  <si>
     <t>US001</t>
   </si>
   <si>
@@ -147,21 +135,12 @@
     <t xml:space="preserve">Quiero darme de alta en el sistemas </t>
   </si>
   <si>
-    <t>Generar mi cuenta de usuario para ingresar al sistema de gestion</t>
-  </si>
-  <si>
     <t xml:space="preserve">Quiero resetear mi clave de usuario </t>
   </si>
   <si>
-    <t xml:space="preserve">Poder ingresar con mi clave nueva al sistema de gestion </t>
-  </si>
-  <si>
     <t>Quiero acceder al sistema de gestion con mi usuario</t>
   </si>
   <si>
-    <t>Poder realizar las gestiones oportunas en el sistema</t>
-  </si>
-  <si>
     <t xml:space="preserve">Modificar una o varias características de un producto ya registrado en el sistema. </t>
   </si>
   <si>
@@ -184,13 +163,106 @@
   </si>
   <si>
     <t>Consultar un producto existente.</t>
+  </si>
+  <si>
+    <t>US0013</t>
+  </si>
+  <si>
+    <t>US0014</t>
+  </si>
+  <si>
+    <t>US0015</t>
+  </si>
+  <si>
+    <t>US0016</t>
+  </si>
+  <si>
+    <t>US0017</t>
+  </si>
+  <si>
+    <t>US0018</t>
+  </si>
+  <si>
+    <t>US0019</t>
+  </si>
+  <si>
+    <t>US0020</t>
+  </si>
+  <si>
+    <t>Como usuario quiero tener un manual de uso de la aplicacion de escritorio.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tener un registro correcto de las ventas realizadas. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modificar uno o varios items de una venta  ya registrado en el sistema. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eliminar una venta que no se ha realizado por algun impedimento </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ingresar con mi clave nueva al sistema de gestion </t>
+  </si>
+  <si>
+    <t>realizar las gestiones oportunas en el sistema</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> aprender el manejo del aplicativo de manera eficaz.</t>
+  </si>
+  <si>
+    <t>tener un registro correcto de las ventas realizadas.</t>
+  </si>
+  <si>
+    <t>generar mi cuenta de usuario para ingresar al sistema de gestion</t>
+  </si>
+  <si>
+    <t>mantenerse un stock de productos actualizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conocer la situacion general del stock </t>
+  </si>
+  <si>
+    <t>mantener un registro de pedidos  actualizado</t>
+  </si>
+  <si>
+    <t>buscar informacion relevante de un producto</t>
+  </si>
+  <si>
+    <t>eliminar stock de un producto determinado</t>
+  </si>
+  <si>
+    <t>manterse un registro de stock actualizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modificar datos de producto con stock minimo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Administrador </t>
+  </si>
+  <si>
+    <t xml:space="preserve">obtener un listado de ventas realizada </t>
+  </si>
+  <si>
+    <t>mantener un registro de las ventas realizadas en un periodo de tiempo</t>
+  </si>
+  <si>
+    <t>obtener un listado de usuarios desactivados del sistema</t>
+  </si>
+  <si>
+    <t>obtener un listado de usuarios no activos en un periodo de tiempo</t>
+  </si>
+  <si>
+    <t>tener el sistema de gestion en funcionamiento en dichas versiones de SO</t>
+  </si>
+  <si>
+    <t>quiero poder ejecutar el sistema de gestion de stock en todas las versiones de Windows, desde Windows 95 en adelante</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -243,6 +315,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -291,7 +369,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -326,6 +404,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,7 +752,7 @@
   <dimension ref="A1:K65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -756,7 +840,7 @@
     </row>
     <row r="6" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -765,7 +849,7 @@
         <v>6</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
@@ -777,16 +861,16 @@
     </row>
     <row r="7" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
@@ -798,16 +882,16 @@
     </row>
     <row r="8" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -819,16 +903,16 @@
     </row>
     <row r="9" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -840,16 +924,16 @@
     </row>
     <row r="10" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>11</v>
+        <v>52</v>
       </c>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -861,16 +945,16 @@
     </row>
     <row r="11" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
@@ -882,16 +966,16 @@
     </row>
     <row r="12" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
@@ -903,16 +987,16 @@
     </row>
     <row r="13" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>7</v>
+        <v>50</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
@@ -924,16 +1008,16 @@
     </row>
     <row r="14" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
@@ -945,16 +1029,16 @@
     </row>
     <row r="15" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -966,16 +1050,16 @@
     </row>
     <row r="16" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
@@ -987,16 +1071,16 @@
     </row>
     <row r="17" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>46</v>
       </c>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
@@ -1007,10 +1091,18 @@
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>47</v>
+      </c>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="4"/>
@@ -1020,10 +1112,18 @@
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="4"/>
@@ -1033,10 +1133,18 @@
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="A20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>42</v>
+      </c>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="4"/>
@@ -1046,10 +1154,18 @@
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>55</v>
+      </c>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
@@ -1059,10 +1175,18 @@
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="A22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>55</v>
+      </c>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
@@ -1072,10 +1196,18 @@
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="A23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D23" s="15" t="s">
+        <v>59</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
@@ -1085,10 +1217,18 @@
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
+      <c r="A24" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="15" t="s">
+        <v>61</v>
+      </c>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
@@ -1098,10 +1238,18 @@
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="A25" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="E25" s="4"/>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
@@ -1125,7 +1273,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>

</xml_diff>